<commit_message>
polishing up the existing EDA
</commit_message>
<xml_diff>
--- a/data/uzbekistan_data.xlsx
+++ b/data/uzbekistan_data.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="185">
   <si>
     <t>Region</t>
   </si>
@@ -516,12 +516,6 @@
   </si>
   <si>
     <t>Republic of Uzbekistan</t>
-  </si>
-  <si>
-    <t>Jizzakh</t>
-  </si>
-  <si>
-    <t>Navoi</t>
   </si>
   <si>
     <t>Population</t>
@@ -5085,7 +5079,7 @@
     </row>
     <row r="3">
       <c r="A3" s="60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="59">
         <v>23.4</v>
@@ -5509,7 +5503,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" s="3">
         <v>2000.0</v>
@@ -5580,7 +5574,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="64">
         <v>10091.0</v>
@@ -5651,7 +5645,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C3" s="66">
         <v>3703.0</v>
@@ -5722,7 +5716,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="66">
         <v>6388.0</v>
@@ -5793,7 +5787,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" s="64">
         <v>741.0</v>
@@ -5864,7 +5858,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" s="66">
         <v>372.0</v>
@@ -5935,7 +5929,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" s="66">
         <v>369.0</v>
@@ -6006,7 +6000,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C8" s="64">
         <v>682.0</v>
@@ -6077,7 +6071,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C9" s="66">
         <v>296.0</v>
@@ -6148,7 +6142,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C10" s="66">
         <v>386.0</v>
@@ -6219,7 +6213,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C11" s="64">
         <v>543.0</v>
@@ -6290,7 +6284,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C12" s="66">
         <v>165.0</v>
@@ -6361,7 +6355,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C13" s="66">
         <v>378.0</v>
@@ -6432,7 +6426,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C14" s="64">
         <v>390.0</v>
@@ -6503,7 +6497,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C15" s="66">
         <v>107.0</v>
@@ -6574,7 +6568,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" s="66">
         <v>283.0</v>
@@ -6645,7 +6639,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" s="64">
         <v>1105.0</v>
@@ -6716,7 +6710,7 @@
         <v>65</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C18" s="64">
         <v>240.0</v>
@@ -6787,7 +6781,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" s="64">
         <v>865.0</v>
@@ -6858,7 +6852,7 @@
         <v>80</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C20" s="66">
         <v>285.0</v>
@@ -6929,7 +6923,7 @@
         <v>80</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C21" s="66">
         <v>135.0</v>
@@ -7000,7 +6994,7 @@
         <v>80</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C22" s="66">
         <v>150.0</v>
@@ -7071,7 +7065,7 @@
         <v>88</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C23" s="64">
         <v>807.0</v>
@@ -7142,7 +7136,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C24" s="66">
         <v>413.0</v>
@@ -7213,7 +7207,7 @@
         <v>88</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C25" s="66">
         <v>394.0</v>
@@ -7284,7 +7278,7 @@
         <v>99</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C26" s="64">
         <v>1000.0</v>
@@ -7355,7 +7349,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="66">
         <v>209.0</v>
@@ -7426,7 +7420,7 @@
         <v>99</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C28" s="66">
         <v>791.0</v>
@@ -7497,7 +7491,7 @@
         <v>106</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C29" s="64">
         <v>930.0</v>
@@ -7568,7 +7562,7 @@
         <v>106</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" s="66">
         <v>168.0</v>
@@ -7639,7 +7633,7 @@
         <v>106</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C31" s="66">
         <v>762.0</v>
@@ -7710,7 +7704,7 @@
         <v>113</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C32" s="64">
         <v>292.0</v>
@@ -7781,7 +7775,7 @@
         <v>113</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C33" s="66">
         <v>86.0</v>
@@ -7852,7 +7846,7 @@
         <v>113</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C34" s="66">
         <v>206.0</v>
@@ -7923,7 +7917,7 @@
         <v>122</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C35" s="64">
         <v>865.0</v>
@@ -7994,7 +7988,7 @@
         <v>122</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C36" s="66">
         <v>313.0</v>
@@ -8065,7 +8059,7 @@
         <v>122</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C37" s="66">
         <v>552.0</v>
@@ -8136,7 +8130,7 @@
         <v>129</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C38" s="64">
         <v>1040.0</v>
@@ -8207,7 +8201,7 @@
         <v>129</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C39" s="66">
         <v>290.0</v>
@@ -8278,7 +8272,7 @@
         <v>129</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C40" s="66">
         <v>750.0</v>
@@ -8349,7 +8343,7 @@
         <v>134</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C41" s="64">
         <v>796.0</v>
@@ -8420,7 +8414,7 @@
         <v>134</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C42" s="66">
         <v>294.0</v>
@@ -8491,7 +8485,7 @@
         <v>134</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C43" s="66">
         <v>502.0</v>
@@ -8562,7 +8556,7 @@
         <v>141</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C44" s="64">
         <v>615.0</v>
@@ -8633,7 +8627,7 @@
         <v>141</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C45" s="66">
         <v>615.0</v>
@@ -8704,7 +8698,7 @@
         <v>141</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -11980,7 +11974,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>180.6</v>
@@ -13543,7 +13537,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>1396.4</v>
@@ -14856,7 +14850,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>211.6</v>
@@ -16437,7 +16431,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>3742.9</v>
@@ -17028,7 +17022,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="64">
         <v>176.0</v>
@@ -18276,8 +18270,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
-        <v>160</v>
+      <c r="A6" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="13">
         <v>24049.0</v>
@@ -18418,8 +18412,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>161</v>
+      <c r="A8" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B8" s="13">
         <v>15305.0</v>
@@ -19171,7 +19165,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="64">
         <v>15.1</v>
@@ -20754,7 +20748,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>833.7</v>
@@ -22335,7 +22329,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>337.3</v>
@@ -22926,7 +22920,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="64">
         <v>17.3</v>
@@ -23909,7 +23903,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>805.0</v>
@@ -25357,7 +25351,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>225.6</v>
@@ -25948,7 +25942,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="64">
         <v>11.5</v>
@@ -26940,7 +26934,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="69">
         <v>613.6</v>
@@ -27531,7 +27525,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="55">
         <v>28.2</v>
@@ -35624,58 +35618,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="G1" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="S1" s="30" t="s">
         <v>177</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="S1" s="30" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2">
@@ -38009,7 +38003,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C8" s="48">
         <v>60.0</v>

</xml_diff>